<commit_message>
More updates before I share the code and initial results.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/USDA GFS IMPACT V16.xlsx
+++ b/data-raw/NutrientData/USDA GFS IMPACT V16.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -2610,8 +2610,8 @@
       <sheetName val="Weighted Composition"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="121">
           <cell r="C121">
@@ -2735,8 +2735,8 @@
       <sheetName val="Weighted Composition"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="382">
           <cell r="C382">
@@ -2860,8 +2860,8 @@
       <sheetName val="Weighted Composition"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="236">
           <cell r="C236">
@@ -2985,8 +2985,8 @@
       <sheetName val="Weighted Composite"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="944">
           <cell r="C944">
@@ -4424,7 +4424,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="BF16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BH3" sqref="BH3"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>